<commit_message>
Parses trainer emails in first sheet of inputted excel file
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4540" yWindow="1200" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Trainers" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Process Suite" sheetId="5" r:id="rId5"/>
     <sheet name="PSA" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -56,22 +56,13 @@
     <t>Kasey Stolba</t>
   </si>
   <si>
-    <t>kstolba@c20g.com</t>
-  </si>
-  <si>
     <t>Daniel Quinn</t>
-  </si>
-  <si>
-    <t>dquinn@c20g.com</t>
   </si>
   <si>
     <t>Intro to Counterpoint</t>
   </si>
   <si>
     <t>Thanh Nguyen</t>
-  </si>
-  <si>
-    <t>tnguyen@c20g.com</t>
   </si>
   <si>
     <t>Front End</t>
@@ -83,16 +74,10 @@
     <t>HTML/DOM</t>
   </si>
   <si>
-    <t>bfoster@c20g.com</t>
-  </si>
-  <si>
     <t>Henry Garrett</t>
   </si>
   <si>
     <t>Intro to Computing</t>
-  </si>
-  <si>
-    <t>hgarrett@c20g.com</t>
   </si>
   <si>
     <t>Tom Crossland</t>
@@ -104,28 +89,16 @@
     <t>Austin Wrenn</t>
   </si>
   <si>
-    <t>awrenn@c20g.com</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
     <t>Andrew Ogilvy</t>
   </si>
   <si>
-    <t>aogilvy@c20g.com</t>
-  </si>
-  <si>
     <t>Ryan Zaki</t>
   </si>
   <si>
-    <t>rzaki@c20g.com</t>
-  </si>
-  <si>
     <t>Ha Ram Yoon</t>
-  </si>
-  <si>
-    <t>hyoon@c20g.com</t>
   </si>
   <si>
     <t>Day 2</t>
@@ -146,13 +119,7 @@
     <t>[Assignment] SQL Basics due</t>
   </si>
   <si>
-    <t>areber@c20g.com</t>
-  </si>
-  <si>
     <t>Kaustubh Soman</t>
-  </si>
-  <si>
-    <t>ksoman@c20g.com</t>
   </si>
   <si>
     <t>Day 3</t>
@@ -167,16 +134,10 @@
     <t>SQL Joins</t>
   </si>
   <si>
-    <t>kkostov@c20g.com</t>
-  </si>
-  <si>
     <t>Tejan Shah</t>
   </si>
   <si>
     <t>SQL Subqueries</t>
-  </si>
-  <si>
-    <t>tshah@c20g.com</t>
   </si>
   <si>
     <t>[Assignment] Aggregate Functions and Joins due</t>
@@ -197,28 +158,16 @@
     <t>[Assignment] Subqueries and Schema Design due</t>
   </si>
   <si>
-    <t>dcollier@c20g.com</t>
-  </si>
-  <si>
     <t>Avery Wauben</t>
   </si>
   <si>
-    <t>awauben@c20g.com</t>
-  </si>
-  <si>
     <t>Ethan Pilot</t>
-  </si>
-  <si>
-    <t>epilot@c20g.com</t>
   </si>
   <si>
     <t>Bootstrap</t>
   </si>
   <si>
     <t>Joe McCormick</t>
-  </si>
-  <si>
-    <t>jmccormick@c20g.com</t>
   </si>
   <si>
     <t>[Assignment] CSS Exercise and Bootstrap due</t>
@@ -484,12 +433,63 @@
     <t>Using generators to create new routable vs non-routable views, contexts, services, and builders
 Purpose of garcon, where and how it is configured</t>
   </si>
+  <si>
+    <t>ta.oracle@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.html@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.javascript@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.jre@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.cordys@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.appworks@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.backbone@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.marionette@c20g.com</t>
+  </si>
+  <si>
+    <t>sql@c20g.com</t>
+  </si>
+  <si>
+    <t>css@c20g.com</t>
+  </si>
+  <si>
+    <t>java@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.mariadb@c20g.com</t>
+  </si>
+  <si>
+    <t>ta.jdk@c20g.com</t>
+  </si>
+  <si>
+    <t>opentext@c20g.com</t>
+  </si>
+  <si>
+    <t>processsuite@c20g.com</t>
+  </si>
+  <si>
+    <t>psa@c20g.com</t>
+  </si>
+  <si>
+    <t>awa@c20g.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -519,6 +519,12 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -551,10 +557,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -592,8 +599,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -930,7 +939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -983,144 +992,163 @@
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
+      <c r="E2" s="19" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>22</v>
+      <c r="E5" s="19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>142</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="D9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="B12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>146</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>59</v>
+        <v>44</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="B15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E12" r:id="rId9"/>
+    <hyperlink ref="E14" r:id="rId10"/>
+    <hyperlink ref="E15" r:id="rId11"/>
+    <hyperlink ref="C5" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="C11" r:id="rId14"/>
+    <hyperlink ref="C12" r:id="rId15"/>
+    <hyperlink ref="C14" r:id="rId16"/>
+    <hyperlink ref="C15" r:id="rId17"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1195,7 +1223,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
@@ -1204,7 +1232,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
@@ -1213,13 +1241,13 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
@@ -1228,7 +1256,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
@@ -1237,7 +1265,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
@@ -1246,13 +1274,13 @@
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
@@ -1261,7 +1289,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
@@ -1270,7 +1298,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1">
@@ -1279,13 +1307,13 @@
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B13" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1">
@@ -4341,7 +4369,7 @@
   </sheetPr>
   <dimension ref="A1:AA981"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
@@ -4399,7 +4427,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
@@ -4408,13 +4436,13 @@
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
@@ -4423,10 +4451,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
@@ -4435,13 +4463,13 @@
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B7" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
@@ -4450,10 +4478,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1">
@@ -4462,13 +4490,13 @@
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B10" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
@@ -4477,10 +4505,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1">
@@ -4489,11 +4517,11 @@
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1">
@@ -4502,13 +4530,13 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1">
@@ -4517,10 +4545,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -4530,16 +4558,16 @@
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B18" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -8451,9 +8479,9 @@
   </sheetPr>
   <dimension ref="A1:AA979"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -8509,7 +8537,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="12"/>
     </row>
@@ -8519,7 +8547,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D3" s="12"/>
     </row>
@@ -8529,7 +8557,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D4" s="12"/>
     </row>
@@ -8541,13 +8569,13 @@
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B6" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12"/>
     </row>
@@ -8557,10 +8585,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
@@ -8571,16 +8599,16 @@
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
@@ -8589,10 +8617,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
@@ -8603,16 +8631,16 @@
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
@@ -8621,10 +8649,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1">
@@ -8635,13 +8663,13 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B15" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D15" s="12"/>
     </row>
@@ -8653,16 +8681,16 @@
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -8673,11 +8701,11 @@
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="10" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D19" s="12"/>
     </row>
@@ -8689,11 +8717,11 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="10" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D21" s="12"/>
     </row>
@@ -8705,16 +8733,16 @@
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B23" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -11639,6 +11667,7 @@
     <hyperlink ref="D23" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -11712,7 +11741,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
@@ -11721,10 +11750,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
@@ -11732,13 +11761,13 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
@@ -11747,16 +11776,16 @@
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B7" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
@@ -11765,13 +11794,13 @@
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B9" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
@@ -11780,16 +11809,16 @@
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B11" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1">
@@ -11798,16 +11827,16 @@
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B13" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1">
@@ -11816,16 +11845,16 @@
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B15" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1">
@@ -11834,16 +11863,16 @@
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B17" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -11852,16 +11881,16 @@
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B19" s="7">
         <v>0.70833333333333337</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -15776,10 +15805,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
@@ -15788,7 +15817,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
@@ -15796,16 +15825,16 @@
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1">
@@ -15814,7 +15843,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
@@ -15823,16 +15852,16 @@
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1">
@@ -15841,7 +15870,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
@@ -15850,16 +15879,16 @@
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1">
@@ -15868,7 +15897,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
@@ -15876,16 +15905,16 @@
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1">
@@ -15894,10 +15923,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1">
@@ -15906,7 +15935,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -15915,16 +15944,16 @@
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B18" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -15933,7 +15962,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -15942,16 +15971,16 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B21" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
@@ -15960,7 +15989,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -15968,13 +15997,13 @@
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B24" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -15983,7 +16012,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -15992,16 +16021,16 @@
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B27" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
@@ -16010,7 +16039,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
@@ -16019,16 +16048,16 @@
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B30" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">

</xml_diff>